<commit_message>
changes for SEIR analysis
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
+++ b/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>beta</t>
   </si>
@@ -29,6 +29,24 @@
   </si>
   <si>
     <t>gamma_inv-min</t>
+  </si>
+  <si>
+    <t>sigma_inv</t>
+  </si>
+  <si>
+    <t>sigma_inv-max</t>
+  </si>
+  <si>
+    <t>sigma_inv-min</t>
+  </si>
+  <si>
+    <t>E_0</t>
+  </si>
+  <si>
+    <t>E_0-max</t>
+  </si>
+  <si>
+    <t>E_0-min</t>
   </si>
   <si>
     <t>R_0</t>
@@ -396,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X4"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -457,6 +475,24 @@
       <c r="R1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" t="s">
+        <v>21</v>
+      </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:24">
       <c r="A2">
@@ -629,19 +665,19 @@
         <v>5</v>
       </c>
       <c r="H4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <v>0.0001</v>
       </c>
       <c r="K4">
-        <v>0.00011</v>
+        <v>0.0001</v>
       </c>
       <c r="L4">
-        <v>9.000000000000001E-05</v>
+        <v>0.0001</v>
       </c>
       <c r="M4">
         <v>2.31</v>
@@ -656,28 +692,102 @@
         <v>108</v>
       </c>
       <c r="Q4">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="R4">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="S4">
         <v>0.1178986076509357</v>
       </c>
       <c r="T4">
-        <v>0.1178984715534684</v>
+        <v>0.1088065509867273</v>
       </c>
       <c r="U4">
-        <v>0.1178862174014433</v>
+        <v>0.1287535821544084</v>
       </c>
       <c r="V4">
         <v>0.8636828726120845</v>
       </c>
       <c r="W4">
-        <v>0.8637388677600084</v>
+        <v>0.8623143049128659</v>
       </c>
       <c r="X4">
-        <v>0.8636197142610648</v>
+        <v>0.8641351461674291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
+      <c r="A5">
+        <v>0.33</v>
+      </c>
+      <c r="B5">
+        <v>0.33</v>
+      </c>
+      <c r="C5">
+        <v>0.33</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>0.0001</v>
+      </c>
+      <c r="K5">
+        <v>0.00015</v>
+      </c>
+      <c r="L5">
+        <v>5E-05</v>
+      </c>
+      <c r="M5">
+        <v>2.31</v>
+      </c>
+      <c r="N5">
+        <v>2.31</v>
+      </c>
+      <c r="O5">
+        <v>2.31</v>
+      </c>
+      <c r="P5">
+        <v>108</v>
+      </c>
+      <c r="Q5">
+        <v>104</v>
+      </c>
+      <c r="R5">
+        <v>115</v>
+      </c>
+      <c r="S5">
+        <v>0.1178986076509357</v>
+      </c>
+      <c r="T5">
+        <v>0.1179499228761208</v>
+      </c>
+      <c r="U5">
+        <v>0.11790579342659</v>
+      </c>
+      <c r="V5">
+        <v>0.8636828726120845</v>
+      </c>
+      <c r="W5">
+        <v>0.863915766140826</v>
+      </c>
+      <c r="X5">
+        <v>0.8632329393796765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes on simulation parameters and plots for SEIR analysis
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
+++ b/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
@@ -748,10 +748,10 @@
         <v>0.0001</v>
       </c>
       <c r="K5">
-        <v>0.00015</v>
+        <v>1E-05</v>
       </c>
       <c r="L5">
-        <v>5E-05</v>
+        <v>0.001</v>
       </c>
       <c r="M5">
         <v>2.31</v>
@@ -766,28 +766,28 @@
         <v>108</v>
       </c>
       <c r="Q5">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="R5">
-        <v>115</v>
+        <v>83</v>
       </c>
       <c r="S5">
         <v>0.1178986076509357</v>
       </c>
       <c r="T5">
-        <v>0.1179499228761208</v>
+        <v>0.1178742211419419</v>
       </c>
       <c r="U5">
-        <v>0.11790579342659</v>
+        <v>0.118437665648738</v>
       </c>
       <c r="V5">
         <v>0.8636828726120845</v>
       </c>
       <c r="W5">
-        <v>0.863915766140826</v>
+        <v>0.8619405466887732</v>
       </c>
       <c r="X5">
-        <v>0.8632329393796765</v>
+        <v>0.8655080918800576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in simulation params
</commit_message>
<xml_diff>
--- a/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
+++ b/results/primer/VanillaSEIR_Scenario0_Primer_200_errorVary.xlsx
@@ -665,10 +665,10 @@
         <v>5</v>
       </c>
       <c r="H4">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="I4">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="J4">
         <v>0.0001</v>
@@ -692,28 +692,28 @@
         <v>108</v>
       </c>
       <c r="Q4">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="R4">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="S4">
         <v>0.1178986076509357</v>
       </c>
       <c r="T4">
-        <v>0.1088065509867273</v>
+        <v>0.1131736743200052</v>
       </c>
       <c r="U4">
-        <v>0.1287535821544084</v>
+        <v>0.1230816648328576</v>
       </c>
       <c r="V4">
         <v>0.8636828726120845</v>
       </c>
       <c r="W4">
-        <v>0.8623143049128659</v>
+        <v>0.8631710361591275</v>
       </c>
       <c r="X4">
-        <v>0.8641351461674291</v>
+        <v>0.8639754189990841</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -748,10 +748,10 @@
         <v>0.0001</v>
       </c>
       <c r="K5">
-        <v>1E-05</v>
+        <v>0.00015</v>
       </c>
       <c r="L5">
-        <v>0.001</v>
+        <v>5E-05</v>
       </c>
       <c r="M5">
         <v>2.31</v>
@@ -766,28 +766,28 @@
         <v>108</v>
       </c>
       <c r="Q5">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="R5">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="S5">
         <v>0.1178986076509357</v>
       </c>
       <c r="T5">
-        <v>0.1178742211419419</v>
+        <v>0.1179499228761208</v>
       </c>
       <c r="U5">
-        <v>0.118437665648738</v>
+        <v>0.11790579342659</v>
       </c>
       <c r="V5">
         <v>0.8636828726120845</v>
       </c>
       <c r="W5">
-        <v>0.8619405466887732</v>
+        <v>0.863915766140826</v>
       </c>
       <c r="X5">
-        <v>0.8655080918800576</v>
+        <v>0.8632329393796765</v>
       </c>
     </row>
   </sheetData>

</xml_diff>